<commit_message>
Run Scripts and Readmes
</commit_message>
<xml_diff>
--- a/datasets/burst_ws/burst_figure_data.xlsx
+++ b/datasets/burst_ws/burst_figure_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmsalamy/Documents/GitHub/james-flumenequi/datasets/burst_ws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08908A87-C62E-2B4C-8AB0-09E7EFA5B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AF2B3F-5CF0-0F40-8A01-33EF2F2A54B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="460" windowWidth="27640" windowHeight="15960" activeTab="3" xr2:uid="{42FB18EF-FB08-504A-A955-FF3F8E9617F4}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15960" activeTab="6" xr2:uid="{42FB18EF-FB08-504A-A955-FF3F8E9617F4}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT" sheetId="2" r:id="rId1"/>
@@ -4475,6 +4475,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6216,7 +6217,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AF97579A-9774-0A4D-8F43-1B2F76E3407B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6227,7 +6228,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F9E79147-88D5-AD4B-9227-CDB3C8C41E7F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6238,7 +6239,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{33BEA069-BBCC-4245-88BF-868AA5871204}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6249,7 +6250,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6282,7 +6283,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6315,7 +6316,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6745,35 +6746,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{FB6ACECA-0DA9-DB4F-B175-DA68495AD708}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_bert_proc" connectionId="5" xr16:uid="{E839D009-8F5E-444E-A0D5-3F41AD4DF106}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{FB6ACECA-0DA9-DB4F-B175-DA68495AD708}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_vgg_proc" connectionId="8" xr16:uid="{40F65D2D-B689-C840-85C6-7C0D801BA6CD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_vgg_proc" connectionId="4" xr16:uid="{736F391A-9B96-DC4F-8B9A-099C3D69A600}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_vgg_proc" connectionId="8" xr16:uid="{40F65D2D-B689-C840-85C6-7C0D801BA6CD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_dn161_proc" connectionId="2" xr16:uid="{4DAB71D3-B6D3-864A-A70F-866C4A54F31D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_dn161_proc" connectionId="6" xr16:uid="{ACA513B5-FD7D-C041-8895-4EC0CB4280BE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_dn161_proc" connectionId="2" xr16:uid="{4DAB71D3-B6D3-864A-A70F-866C4A54F31D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="3" xr16:uid="{96A7DB28-2029-044C-8753-4C58BE8499D3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="7" xr16:uid="{EEB871FD-00EC-1346-83FA-16DD26D3E36F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="7" xr16:uid="{EEB871FD-00EC-1346-83FA-16DD26D3E36F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="3" xr16:uid="{96A7DB28-2029-044C-8753-4C58BE8499D3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11222,7 +11223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1001B085-9B2E-3648-946A-D57EFD197ECF}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23:H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Scripts and Readme Files
</commit_message>
<xml_diff>
--- a/datasets/burst_ws/burst_figure_data.xlsx
+++ b/datasets/burst_ws/burst_figure_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmsalamy/Documents/GitHub/james-flumenequi/datasets/burst_ws/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08908A87-C62E-2B4C-8AB0-09E7EFA5B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AF2B3F-5CF0-0F40-8A01-33EF2F2A54B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="460" windowWidth="27640" windowHeight="15960" activeTab="3" xr2:uid="{42FB18EF-FB08-504A-A955-FF3F8E9617F4}"/>
+    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15960" activeTab="6" xr2:uid="{42FB18EF-FB08-504A-A955-FF3F8E9617F4}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT" sheetId="2" r:id="rId1"/>
@@ -4475,6 +4475,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -6216,7 +6217,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{AF97579A-9774-0A4D-8F43-1B2F76E3407B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6227,7 +6228,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F9E79147-88D5-AD4B-9227-CDB3C8C41E7F}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6238,7 +6239,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{33BEA069-BBCC-4245-88BF-868AA5871204}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="120" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="114" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6249,7 +6250,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6282,7 +6283,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6315,7 +6316,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6064250"/>
+    <xdr:ext cx="9302193" cy="6060351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6745,35 +6746,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{FB6ACECA-0DA9-DB4F-B175-DA68495AD708}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_bert_proc" connectionId="5" xr16:uid="{E839D009-8F5E-444E-A0D5-3F41AD4DF106}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_bert_proc" connectionId="1" xr16:uid="{FB6ACECA-0DA9-DB4F-B175-DA68495AD708}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_vgg_proc" connectionId="8" xr16:uid="{40F65D2D-B689-C840-85C6-7C0D801BA6CD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_vgg_proc" connectionId="4" xr16:uid="{736F391A-9B96-DC4F-8B9A-099C3D69A600}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_vgg_proc" connectionId="8" xr16:uid="{40F65D2D-B689-C840-85C6-7C0D801BA6CD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_dn161_proc" connectionId="2" xr16:uid="{4DAB71D3-B6D3-864A-A70F-866C4A54F31D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_dn161_proc" connectionId="6" xr16:uid="{ACA513B5-FD7D-C041-8895-4EC0CB4280BE}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_dn161_proc" connectionId="2" xr16:uid="{4DAB71D3-B6D3-864A-A70F-866C4A54F31D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="3" xr16:uid="{96A7DB28-2029-044C-8753-4C58BE8499D3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="7" xr16:uid="{EEB871FD-00EC-1346-83FA-16DD26D3E36F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tcp_burst_r50_proc" connectionId="7" xr16:uid="{EEB871FD-00EC-1346-83FA-16DD26D3E36F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="iter_burst_r50_proc" connectionId="3" xr16:uid="{96A7DB28-2029-044C-8753-4C58BE8499D3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11222,7 +11223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1001B085-9B2E-3648-946A-D57EFD197ECF}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23:H29"/>
     </sheetView>
   </sheetViews>

</xml_diff>